<commit_message>
Updated NGIN latest code
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_NGIN.xlsx
+++ b/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_NGIN.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="252">
   <si>
     <t>ExistingOrderNumber</t>
   </si>
@@ -204,15 +204,9 @@
     <t>ChangeOrder_VoicelineNumber</t>
   </si>
   <si>
-    <t>NGIN_</t>
-  </si>
-  <si>
     <t>BE (Belgium)</t>
   </si>
   <si>
-    <t>NGINUser</t>
-  </si>
-  <si>
     <t>Chennai</t>
   </si>
   <si>
@@ -267,9 +261,6 @@
     <t>Reseller_Fax</t>
   </si>
   <si>
-    <t>nginreseller18@gmail.com</t>
-  </si>
-  <si>
     <t>Pondicherry</t>
   </si>
   <si>
@@ -279,15 +270,6 @@
     <t>35</t>
   </si>
   <si>
-    <t>87653</t>
-  </si>
-  <si>
-    <t>875473</t>
-  </si>
-  <si>
-    <t>9976856437</t>
-  </si>
-  <si>
     <t>Reseller_EditEmail</t>
   </si>
   <si>
@@ -312,9 +294,6 @@
     <t>Reseller_EditFax</t>
   </si>
   <si>
-    <t>nginreselleredit18@gmail.com</t>
-  </si>
-  <si>
     <t>Pondi</t>
   </si>
   <si>
@@ -324,15 +303,6 @@
     <t>37</t>
   </si>
   <si>
-    <t>87698</t>
-  </si>
-  <si>
-    <t>925473</t>
-  </si>
-  <si>
-    <t>9976856426</t>
-  </si>
-  <si>
     <t>Customer_Country</t>
   </si>
   <si>
@@ -405,9 +375,6 @@
     <t>Reseller_EditResellerName</t>
   </si>
   <si>
-    <t>Reselleredit18</t>
-  </si>
-  <si>
     <t>ServiceProfile</t>
   </si>
   <si>
@@ -444,72 +411,6 @@
     <t>DEFAULT</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>NGIN_19</t>
-  </si>
-  <si>
-    <t>ngindomain19.com</t>
-  </si>
-  <si>
-    <t>nginocn19</t>
-  </si>
-  <si>
-    <t>testreference19</t>
-  </si>
-  <si>
-    <t>ngincontact19</t>
-  </si>
-  <si>
-    <t>ngin19@test.com</t>
-  </si>
-  <si>
-    <t>9876894548</t>
-  </si>
-  <si>
-    <t>1987765</t>
-  </si>
-  <si>
-    <t>NGINOrder_19</t>
-  </si>
-  <si>
-    <t>NGINRFI_19</t>
-  </si>
-  <si>
-    <t>NGINUser_19</t>
-  </si>
-  <si>
-    <t>User_19</t>
-  </si>
-  <si>
-    <t>NGINUser_19@gmail.com</t>
-  </si>
-  <si>
-    <t>9643745668</t>
-  </si>
-  <si>
-    <t>NGINUser19</t>
-  </si>
-  <si>
-    <t>User19</t>
-  </si>
-  <si>
-    <t>NGIN19@gmail.com</t>
-  </si>
-  <si>
-    <t>NGINOrderedit_19</t>
-  </si>
-  <si>
-    <t>NGINRFIedit_19</t>
-  </si>
-  <si>
-    <t>9856736498</t>
-  </si>
-  <si>
-    <t>Reseller19</t>
-  </si>
-  <si>
     <t>C:\\Users\\SSUPRAJA-adm\\Downloads</t>
   </si>
   <si>
@@ -531,18 +432,6 @@
     <t>SANNumberValue</t>
   </si>
   <si>
-    <t>InternationalOutgoingCalls_checkedvalue</t>
-  </si>
-  <si>
-    <t>InternationalIncomingCalls_checkedvalue</t>
-  </si>
-  <si>
-    <t>MobileCallsAllowed_checkedvalue</t>
-  </si>
-  <si>
-    <t>PayphoneBlockingenabled_checkedvalue</t>
-  </si>
-  <si>
     <t>Supervisionfieldvalue</t>
   </si>
   <si>
@@ -552,9 +441,6 @@
     <t>CPSFreeFormatValue</t>
   </si>
   <si>
-    <t>WebAccessBlockedvalue</t>
-  </si>
-  <si>
     <t>Full (2)</t>
   </si>
   <si>
@@ -564,18 +450,6 @@
     <t>NGINMessage_SANNumber</t>
   </si>
   <si>
-    <t>390200620891</t>
-  </si>
-  <si>
-    <t>SANBlockEnabled_Checkedvalue</t>
-  </si>
-  <si>
-    <t>FOCEnabled_Checkedvalue</t>
-  </si>
-  <si>
-    <t>EnablePriceAnnouncement_Checkedvalue</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
@@ -591,9 +465,6 @@
     <t>FR-nginocn10</t>
   </si>
   <si>
-    <t>NGINService_2105</t>
-  </si>
-  <si>
     <t>AddSAN_SANNumber</t>
   </si>
   <si>
@@ -705,9 +576,6 @@
     <t>Edit_NumberOfRepetitionsAllowedValue</t>
   </si>
   <si>
-    <t>14438932</t>
-  </si>
-  <si>
     <t>9854352787</t>
   </si>
   <si>
@@ -717,10 +585,196 @@
     <t>14498738</t>
   </si>
   <si>
-    <t>3314456823</t>
-  </si>
-  <si>
     <t>ExistingOrderService</t>
+  </si>
+  <si>
+    <t>NGINUseredit</t>
+  </si>
+  <si>
+    <t>623183</t>
+  </si>
+  <si>
+    <t>875642</t>
+  </si>
+  <si>
+    <t>9973738994</t>
+  </si>
+  <si>
+    <t>9973726713</t>
+  </si>
+  <si>
+    <t>82673</t>
+  </si>
+  <si>
+    <t>978292</t>
+  </si>
+  <si>
+    <t>9972654372</t>
+  </si>
+  <si>
+    <t>9976763093</t>
+  </si>
+  <si>
+    <t>3314498738</t>
+  </si>
+  <si>
+    <t>InternationalOutgoingCalls_checkbox</t>
+  </si>
+  <si>
+    <t>InternationalIncomingCalls_checkbox</t>
+  </si>
+  <si>
+    <t>MobileCallsAllowed_checkbox</t>
+  </si>
+  <si>
+    <t>PayphoneBlockingenabled_checkbox</t>
+  </si>
+  <si>
+    <t>WebAccessBlocked_checkbox</t>
+  </si>
+  <si>
+    <t>SANBlock_Checkbox</t>
+  </si>
+  <si>
+    <t>FOCEnabled_Checkbox</t>
+  </si>
+  <si>
+    <t>EnableLogicalRouting_Checkbox</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Edit_ServiceProfile</t>
+  </si>
+  <si>
+    <t>Edit_SupervisionValue</t>
+  </si>
+  <si>
+    <t>Edit_InternationalOutgoingCalls_checkbox</t>
+  </si>
+  <si>
+    <t>Edit_InternationalIncomingCalls_checkbox</t>
+  </si>
+  <si>
+    <t>Edit_MobileCallsAllowed_checkbox</t>
+  </si>
+  <si>
+    <t>Edit_NoReplyTimerValue</t>
+  </si>
+  <si>
+    <t>Edit_MaxCallDuration</t>
+  </si>
+  <si>
+    <t>Edit_PayphoneBlockingenabled_checkbox</t>
+  </si>
+  <si>
+    <t>Edit_WebAccessBlocked_checkbox</t>
+  </si>
+  <si>
+    <t>Edit_SANBlock_Checkbox</t>
+  </si>
+  <si>
+    <t>Edit_FOCEnabled_Checkbox</t>
+  </si>
+  <si>
+    <t>Edit_RingToNumber_Checkbox</t>
+  </si>
+  <si>
+    <t>Edit_AnnouncementToPlay_Checkbox</t>
+  </si>
+  <si>
+    <t>Edit_ComplexRouting_Checkbox</t>
+  </si>
+  <si>
+    <t>Edit_PreDestinationNumber</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>NGIN2106</t>
+  </si>
+  <si>
+    <t>ngindomain2106.com</t>
+  </si>
+  <si>
+    <t>nginocn2106</t>
+  </si>
+  <si>
+    <t>testreference2106</t>
+  </si>
+  <si>
+    <t>ngincontact2106</t>
+  </si>
+  <si>
+    <t>ngin2106@test.com</t>
+  </si>
+  <si>
+    <t>NGINOrder_2106</t>
+  </si>
+  <si>
+    <t>NGINRFI_2106</t>
+  </si>
+  <si>
+    <t>NGINService_2106</t>
+  </si>
+  <si>
+    <t>NGINUser_2106</t>
+  </si>
+  <si>
+    <t>User_2106</t>
+  </si>
+  <si>
+    <t>NGINUser_2106@gmail.com</t>
+  </si>
+  <si>
+    <t>NGINUseredit2106</t>
+  </si>
+  <si>
+    <t>Useredit2106</t>
+  </si>
+  <si>
+    <t>NGINUseredit_2106@gmail.com</t>
+  </si>
+  <si>
+    <t>NGINOrderedit_2106</t>
+  </si>
+  <si>
+    <t>NGINRFIedit_2106</t>
+  </si>
+  <si>
+    <t>nginreseller2106@gmail.com</t>
+  </si>
+  <si>
+    <t>nginreselleredit2106@gmail.com</t>
+  </si>
+  <si>
+    <t>Reseller2106</t>
+  </si>
+  <si>
+    <t>Reselleredit2106</t>
+  </si>
+  <si>
+    <t>FR-nginocn2106</t>
+  </si>
+  <si>
+    <t>390202106891</t>
+  </si>
+  <si>
+    <t>9876837238</t>
+  </si>
+  <si>
+    <t>3892753</t>
+  </si>
+  <si>
+    <t>9643202738</t>
+  </si>
+  <si>
+    <t>9856372451</t>
+  </si>
+  <si>
+    <t>3314785453</t>
   </si>
 </sst>
 </file>
@@ -799,7 +853,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,6 +872,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1099,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EM2"/>
+  <dimension ref="A1:FD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1133,9 +1190,18 @@
     <col min="32" max="33" width="12.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="34" max="34" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="16.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="41" width="9.140625" style="2" collapsed="1"/>
+    <col min="36" max="38" width="9.140625" style="2" collapsed="1"/>
+    <col min="39" max="39" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="41" width="9.140625" style="2" collapsed="1"/>
     <col min="42" max="42" width="26.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="51" width="9.140625" style="2" collapsed="1"/>
+    <col min="43" max="43" width="14.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="45" width="9.140625" style="2" collapsed="1"/>
+    <col min="46" max="46" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="19" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="11" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="22.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="19.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="9.140625" style="2" collapsed="1"/>
     <col min="52" max="52" width="23.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="53" max="53" width="26.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="54" max="54" width="26.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1184,7 +1250,7 @@
     <col min="101" max="101" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="102" max="103" width="25.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="104" max="104" width="19.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="105" max="105" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="21.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="106" max="106" width="25.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="107" max="107" width="19.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="108" max="108" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1193,7 +1259,7 @@
     <col min="112" max="112" width="24.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="113" max="113" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="114" max="114" width="36.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="115" max="115" width="18.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="115" width="20.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="116" max="116" width="30.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="117" max="117" width="26.140625" style="2" customWidth="1" collapsed="1"/>
     <col min="118" max="118" width="39.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1218,10 +1284,12 @@
     <col min="141" max="141" width="42.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="142" max="142" width="32.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="143" max="143" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="144" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="144" max="144" width="30.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="145" max="145" width="25.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="146" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143">
+    <row r="1" spans="1:160">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1274,7 +1342,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>31</v>
@@ -1340,7 +1408,7 @@
         <v>48</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>14</v>
@@ -1367,13 +1435,13 @@
         <v>56</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>57</v>
@@ -1388,306 +1456,357 @@
         <v>60</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BF1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="BH1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CG1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="BI1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BZ1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CT1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EP1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="ER1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="CE1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="CF1" s="1" t="s">
+      <c r="ES1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="CI1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="EW1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="EY1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="FA1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="FB1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="CN1" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DB1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="DM1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="DU1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="EB1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="ED1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="EE1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="EF1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="EH1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="EI1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:160">
+      <c r="A2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="EM1" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:143">
-      <c r="A2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>146</v>
+        <v>228</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>147</v>
+        <v>229</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>5</v>
@@ -1702,7 +1821,7 @@
         <v>22</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>5</v>
@@ -1711,22 +1830,22 @@
         <v>6</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>25</v>
@@ -1759,10 +1878,10 @@
         <v>44</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>153</v>
+        <v>234</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>26</v>
@@ -1771,31 +1890,31 @@
         <v>49</v>
       </c>
       <c r="AN2" s="5" t="s">
-        <v>154</v>
+        <v>235</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>156</v>
+        <v>236</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>157</v>
+        <v>237</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="AT2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>158</v>
+        <v>238</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>6</v>
@@ -1804,142 +1923,142 @@
         <v>5</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>159</v>
+        <v>239</v>
       </c>
       <c r="BA2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="BF2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BH2" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="BB2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="BF2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="BI2" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BL2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BJ2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BL2" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="BM2" s="2" t="s">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BQ2" s="5" t="s">
-        <v>97</v>
+        <v>242</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="BT2" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="BU2" s="2" t="s">
-        <v>101</v>
+        <v>194</v>
       </c>
       <c r="BV2" s="2" t="s">
-        <v>102</v>
+        <v>195</v>
       </c>
       <c r="BW2" s="2" t="s">
-        <v>103</v>
+        <v>196</v>
       </c>
       <c r="BX2" s="2" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="BY2" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="CA2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="CB2" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="CC2" t="s">
         <v>162</v>
       </c>
-      <c r="BZ2" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="CA2" s="8" t="s">
+      <c r="CD2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>146</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>140</v>
+      </c>
+      <c r="CI2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CK2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CL2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CM2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CN2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="CO2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="CP2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="CQ2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="CB2" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>188</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>178</v>
-      </c>
-      <c r="CI2" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CK2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CL2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CM2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CN2" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="CO2" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="CP2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="CQ2" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="CR2" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="CS2" s="2" t="s">
         <v>6</v>
@@ -1951,145 +2070,196 @@
         <v>5</v>
       </c>
       <c r="CV2" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="CW2" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="CX2" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="CY2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DA2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>146</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DF2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DH2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DI2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DJ2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="DK2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DL2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="DM2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DP2" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="DQ2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="DR2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="DS2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>153</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>152</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>98</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>147</v>
+      </c>
+      <c r="DX2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="DY2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="CZ2" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="DA2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DB2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>196</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>195</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>108</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>189</v>
-      </c>
-      <c r="DG2" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="DH2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="DI2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="DJ2" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="DK2" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="DL2" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="DM2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="DN2" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="DO2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="DP2" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="DQ2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="DR2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="DS2" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="DT2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DU2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DV2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DW2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DX2" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DY2" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="DZ2" s="2" t="s">
-        <v>205</v>
+        <v>129</v>
       </c>
       <c r="EA2" s="2" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="EB2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="EC2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="ED2" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="EE2" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="EF2" s="2" t="s">
-        <v>205</v>
+        <v>131</v>
+      </c>
+      <c r="EC2" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>245</v>
+      </c>
+      <c r="EE2" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="EF2" s="8" t="s">
+        <v>246</v>
       </c>
       <c r="EG2" s="2" t="s">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="EH2" s="2" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="EI2" s="2" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
       <c r="EJ2" s="2" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="EK2" s="2" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="EL2" s="2" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="EM2" s="2" t="s">
-        <v>205</v>
+        <v>162</v>
+      </c>
+      <c r="EN2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EO2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EP2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EQ2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="ER2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="ES2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="ET2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="EU2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="EV2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="EW2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EX2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EY2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="EZ2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="FA2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="FB2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="FC2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="FD2" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AN2" r:id="rId1"/>
-    <hyperlink ref="AU2" r:id="rId2"/>
-    <hyperlink ref="J2" r:id="rId3"/>
-    <hyperlink ref="BI2" r:id="rId4"/>
-    <hyperlink ref="BQ2" r:id="rId5"/>
+    <hyperlink ref="AN2" r:id="rId1" display="NGINUser_1306@gmail.com"/>
+    <hyperlink ref="AU2" r:id="rId2" display="NGINUseredit_1306@gmail.com"/>
+    <hyperlink ref="J2" r:id="rId3" display="ngin1306@test.com"/>
+    <hyperlink ref="BI2" r:id="rId4" display="nginreseller1306@gmail.com"/>
+    <hyperlink ref="BQ2" r:id="rId5" display="nginreselleredit1306@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
NGIN data sheet updated
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_NGIN.xlsx
+++ b/APTAutomationProject/src/com/saksoft/qa/datalibrary/APT_NGIN.xlsx
@@ -582,9 +582,6 @@
     <t>87684</t>
   </si>
   <si>
-    <t>14498738</t>
-  </si>
-  <si>
     <t>ExistingOrderService</t>
   </si>
   <si>
@@ -693,75 +690,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>NGIN2106</t>
-  </si>
-  <si>
-    <t>ngindomain2106.com</t>
-  </si>
-  <si>
-    <t>nginocn2106</t>
-  </si>
-  <si>
-    <t>testreference2106</t>
-  </si>
-  <si>
-    <t>ngincontact2106</t>
-  </si>
-  <si>
-    <t>ngin2106@test.com</t>
-  </si>
-  <si>
-    <t>NGINOrder_2106</t>
-  </si>
-  <si>
-    <t>NGINRFI_2106</t>
-  </si>
-  <si>
-    <t>NGINService_2106</t>
-  </si>
-  <si>
-    <t>NGINUser_2106</t>
-  </si>
-  <si>
-    <t>User_2106</t>
-  </si>
-  <si>
-    <t>NGINUser_2106@gmail.com</t>
-  </si>
-  <si>
-    <t>NGINUseredit2106</t>
-  </si>
-  <si>
-    <t>Useredit2106</t>
-  </si>
-  <si>
-    <t>NGINUseredit_2106@gmail.com</t>
-  </si>
-  <si>
-    <t>NGINOrderedit_2106</t>
-  </si>
-  <si>
-    <t>NGINRFIedit_2106</t>
-  </si>
-  <si>
-    <t>nginreseller2106@gmail.com</t>
-  </si>
-  <si>
-    <t>nginreselleredit2106@gmail.com</t>
-  </si>
-  <si>
-    <t>Reseller2106</t>
-  </si>
-  <si>
-    <t>Reselleredit2106</t>
-  </si>
-  <si>
-    <t>FR-nginocn2106</t>
-  </si>
-  <si>
-    <t>390202106891</t>
-  </si>
-  <si>
     <t>9876837238</t>
   </si>
   <si>
@@ -775,6 +703,78 @@
   </si>
   <si>
     <t>3314785453</t>
+  </si>
+  <si>
+    <t>NGIN2906</t>
+  </si>
+  <si>
+    <t>ngindomain2906.com</t>
+  </si>
+  <si>
+    <t>nginocn2906</t>
+  </si>
+  <si>
+    <t>testreference2906</t>
+  </si>
+  <si>
+    <t>ngincontact2906</t>
+  </si>
+  <si>
+    <t>ngin2906@test.com</t>
+  </si>
+  <si>
+    <t>NGINOrder_2906</t>
+  </si>
+  <si>
+    <t>NGINRFI_2906</t>
+  </si>
+  <si>
+    <t>NGINService_2906</t>
+  </si>
+  <si>
+    <t>NGINUser_2906</t>
+  </si>
+  <si>
+    <t>User_2906</t>
+  </si>
+  <si>
+    <t>NGINUser_2906@gmail.com</t>
+  </si>
+  <si>
+    <t>NGINUseredit2906</t>
+  </si>
+  <si>
+    <t>Useredit2906</t>
+  </si>
+  <si>
+    <t>NGINUseredit_2906@gmail.com</t>
+  </si>
+  <si>
+    <t>NGINOrderedit_2906</t>
+  </si>
+  <si>
+    <t>NGINRFIedit_2906</t>
+  </si>
+  <si>
+    <t>nginreseller2906@gmail.com</t>
+  </si>
+  <si>
+    <t>nginreselleredit2906@gmail.com</t>
+  </si>
+  <si>
+    <t>Reseller2906</t>
+  </si>
+  <si>
+    <t>Reselleredit2906</t>
+  </si>
+  <si>
+    <t>FR-nginocn2906</t>
+  </si>
+  <si>
+    <t>390202906891</t>
+  </si>
+  <si>
+    <t>14498278</t>
   </si>
 </sst>
 </file>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="DX1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DZ5" sqref="DZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1267,7 +1267,7 @@
     <col min="121" max="122" width="28.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="123" max="123" width="41.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="124" max="124" width="35.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="125" max="125" width="12.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="125" max="125" width="18.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="126" max="127" width="18" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="128" max="128" width="34.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="129" max="129" width="37.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1342,7 +1342,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>31</v>
@@ -1534,16 +1534,16 @@
         <v>101</v>
       </c>
       <c r="CD1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="CE1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="CH1" s="1" t="s">
         <v>137</v>
@@ -1552,13 +1552,13 @@
         <v>138</v>
       </c>
       <c r="CJ1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="CK1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>163</v>
@@ -1597,55 +1597,55 @@
         <v>115</v>
       </c>
       <c r="CY1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CZ1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="DA1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="DF1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="DF1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="DJ1" s="1" t="s">
         <v>177</v>
       </c>
       <c r="DK1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="DL1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="DM1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="DP1" s="1" t="s">
         <v>117</v>
@@ -1773,40 +1773,40 @@
     </row>
     <row r="2" spans="1:160">
       <c r="A2" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>5</v>
@@ -1821,7 +1821,7 @@
         <v>22</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>5</v>
@@ -1830,22 +1830,22 @@
         <v>6</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>25</v>
@@ -1878,10 +1878,10 @@
         <v>44</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>26</v>
@@ -1890,31 +1890,31 @@
         <v>49</v>
       </c>
       <c r="AN2" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>62</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="AW2" s="2" t="s">
         <v>6</v>
@@ -1926,16 +1926,16 @@
         <v>98</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="BD2" s="2" t="s">
         <v>65</v>
@@ -1953,7 +1953,7 @@
         <v>160</v>
       </c>
       <c r="BI2" s="5" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BJ2" s="2" t="s">
         <v>80</v>
@@ -1965,19 +1965,19 @@
         <v>82</v>
       </c>
       <c r="BM2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BN2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BP2" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="BP2" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="BQ2" s="5" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="BR2" s="2" t="s">
         <v>91</v>
@@ -1989,22 +1989,22 @@
         <v>93</v>
       </c>
       <c r="BU2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="BV2" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BW2" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="BW2" s="2" t="s">
+      <c r="BX2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="BX2" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="BY2" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="BZ2" s="2" t="s">
-        <v>187</v>
+        <v>251</v>
       </c>
       <c r="CA2" s="8" t="s">
         <v>144</v>
@@ -2046,7 +2046,7 @@
         <v>69</v>
       </c>
       <c r="CN2" s="9" t="s">
-        <v>187</v>
+        <v>251</v>
       </c>
       <c r="CO2" s="2" t="s">
         <v>185</v>
@@ -2079,7 +2079,7 @@
         <v>116</v>
       </c>
       <c r="CY2" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="CZ2" s="2" t="s">
         <v>162</v>
@@ -2130,7 +2130,7 @@
         <v>162</v>
       </c>
       <c r="DP2" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="DQ2" s="2" t="s">
         <v>141</v>
@@ -2169,16 +2169,16 @@
         <v>131</v>
       </c>
       <c r="EC2" s="10" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="ED2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="EE2" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="EF2" s="8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="EG2" s="2" t="s">
         <v>151</v>

</xml_diff>